<commit_message>
feature : assemble siae frequency
</commit_message>
<xml_diff>
--- a/03-WTP-PoC/code/apps/spectrum/exl2cmd/NextFrequency.xlsx
+++ b/03-WTP-PoC/code/apps/spectrum/exl2cmd/NextFrequency.xlsx
@@ -74,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,15 +116,11 @@
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="0"/>
       <charset val="1"/>
@@ -151,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -211,13 +207,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -293,31 +282,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,14 +389,14 @@
   </sheetPr>
   <dimension ref="B2:AMJ65535"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z12" activeCellId="0" sqref="Z12:AA24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V22" activeCellId="0" sqref="V22:W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.53023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.1906976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.61860465116279"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3720930232558"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,18 +603,18 @@
         <v>5960025</v>
       </c>
       <c r="T4" s="5" t="n">
-        <v>72125000</v>
+        <v>71375000</v>
       </c>
       <c r="U4" s="6" t="n">
-        <v>82125000</v>
+        <v>81375000</v>
       </c>
       <c r="V4" s="7" t="n">
         <f aca="false">U4</f>
-        <v>82125000</v>
+        <v>81375000</v>
       </c>
       <c r="W4" s="8" t="n">
         <f aca="false">T4</f>
-        <v>72125000</v>
+        <v>71375000</v>
       </c>
       <c r="X4" s="5" t="n">
         <v>11205000</v>
@@ -716,19 +705,19 @@
       </c>
       <c r="T5" s="5" t="n">
         <f aca="false">T4+250000</f>
-        <v>72375000</v>
+        <v>71625000</v>
       </c>
       <c r="U5" s="6" t="n">
         <f aca="false">U4+250000</f>
-        <v>82375000</v>
+        <v>81625000</v>
       </c>
       <c r="V5" s="7" t="n">
         <f aca="false">U5</f>
-        <v>82375000</v>
+        <v>81625000</v>
       </c>
       <c r="W5" s="8" t="n">
         <f aca="false">T5</f>
-        <v>72375000</v>
+        <v>71625000</v>
       </c>
       <c r="X5" s="5" t="n">
         <f aca="false">X4+25000</f>
@@ -820,19 +809,19 @@
       </c>
       <c r="T6" s="5" t="n">
         <f aca="false">T5+250000</f>
-        <v>72625000</v>
+        <v>71875000</v>
       </c>
       <c r="U6" s="6" t="n">
         <f aca="false">U5+250000</f>
-        <v>82625000</v>
+        <v>81875000</v>
       </c>
       <c r="V6" s="7" t="n">
         <f aca="false">U6</f>
-        <v>82625000</v>
+        <v>81875000</v>
       </c>
       <c r="W6" s="8" t="n">
         <f aca="false">T6</f>
-        <v>72625000</v>
+        <v>71875000</v>
       </c>
       <c r="X6" s="5" t="n">
         <f aca="false">X5+25000</f>
@@ -918,19 +907,19 @@
       </c>
       <c r="T7" s="5" t="n">
         <f aca="false">T6+250000</f>
-        <v>72875000</v>
+        <v>72125000</v>
       </c>
       <c r="U7" s="6" t="n">
         <f aca="false">U6+250000</f>
-        <v>82875000</v>
+        <v>82125000</v>
       </c>
       <c r="V7" s="7" t="n">
         <f aca="false">U7</f>
-        <v>82875000</v>
+        <v>82125000</v>
       </c>
       <c r="W7" s="8" t="n">
         <f aca="false">T7</f>
-        <v>72875000</v>
+        <v>72125000</v>
       </c>
       <c r="X7" s="5" t="n">
         <f aca="false">X6+25000</f>
@@ -1006,19 +995,19 @@
       <c r="S8" s="8"/>
       <c r="T8" s="5" t="n">
         <f aca="false">T7+250000</f>
-        <v>73125000</v>
+        <v>72375000</v>
       </c>
       <c r="U8" s="6" t="n">
         <f aca="false">U7+250000</f>
-        <v>83125000</v>
+        <v>82375000</v>
       </c>
       <c r="V8" s="7" t="n">
         <f aca="false">U8</f>
-        <v>83125000</v>
+        <v>82375000</v>
       </c>
       <c r="W8" s="8" t="n">
         <f aca="false">T8</f>
-        <v>73125000</v>
+        <v>72375000</v>
       </c>
       <c r="X8" s="5" t="n">
         <f aca="false">X7+25000</f>
@@ -1094,19 +1083,19 @@
       <c r="S9" s="8"/>
       <c r="T9" s="5" t="n">
         <f aca="false">T8+250000</f>
-        <v>73375000</v>
+        <v>72625000</v>
       </c>
       <c r="U9" s="6" t="n">
         <f aca="false">U8+250000</f>
-        <v>83375000</v>
+        <v>82625000</v>
       </c>
       <c r="V9" s="7" t="n">
         <f aca="false">U9</f>
-        <v>83375000</v>
+        <v>82625000</v>
       </c>
       <c r="W9" s="8" t="n">
         <f aca="false">T9</f>
-        <v>73375000</v>
+        <v>72625000</v>
       </c>
       <c r="X9" s="5" t="n">
         <f aca="false">X8+25000</f>
@@ -1182,19 +1171,19 @@
       <c r="S10" s="8"/>
       <c r="T10" s="5" t="n">
         <f aca="false">T9+250000</f>
-        <v>73625000</v>
+        <v>72875000</v>
       </c>
       <c r="U10" s="6" t="n">
         <f aca="false">U9+250000</f>
-        <v>83625000</v>
+        <v>82875000</v>
       </c>
       <c r="V10" s="7" t="n">
         <f aca="false">U10</f>
-        <v>83625000</v>
+        <v>82875000</v>
       </c>
       <c r="W10" s="8" t="n">
         <f aca="false">T10</f>
-        <v>73625000</v>
+        <v>72875000</v>
       </c>
       <c r="X10" s="5" t="n">
         <f aca="false">X9+25000</f>
@@ -1270,19 +1259,19 @@
       <c r="S11" s="8"/>
       <c r="T11" s="5" t="n">
         <f aca="false">T10+250000</f>
-        <v>73875000</v>
+        <v>73125000</v>
       </c>
       <c r="U11" s="6" t="n">
         <f aca="false">U10+250000</f>
-        <v>83875000</v>
+        <v>83125000</v>
       </c>
       <c r="V11" s="7" t="n">
         <f aca="false">U11</f>
-        <v>83875000</v>
+        <v>83125000</v>
       </c>
       <c r="W11" s="8" t="n">
         <f aca="false">T11</f>
-        <v>73875000</v>
+        <v>73125000</v>
       </c>
       <c r="X11" s="5" t="n">
         <f aca="false">X10+25000</f>
@@ -1358,19 +1347,19 @@
       <c r="S12" s="8"/>
       <c r="T12" s="5" t="n">
         <f aca="false">T11+250000</f>
-        <v>74125000</v>
+        <v>73375000</v>
       </c>
       <c r="U12" s="6" t="n">
         <f aca="false">U11+250000</f>
-        <v>84125000</v>
+        <v>83375000</v>
       </c>
       <c r="V12" s="7" t="n">
         <f aca="false">U12</f>
-        <v>84125000</v>
+        <v>83375000</v>
       </c>
       <c r="W12" s="8" t="n">
         <f aca="false">T12</f>
-        <v>74125000</v>
+        <v>73375000</v>
       </c>
       <c r="X12" s="5"/>
       <c r="Y12" s="6"/>
@@ -1434,19 +1423,19 @@
       <c r="S13" s="8"/>
       <c r="T13" s="5" t="n">
         <f aca="false">T12+250000</f>
-        <v>74375000</v>
+        <v>73625000</v>
       </c>
       <c r="U13" s="6" t="n">
         <f aca="false">U12+250000</f>
-        <v>84375000</v>
+        <v>83625000</v>
       </c>
       <c r="V13" s="7" t="n">
         <f aca="false">U13</f>
-        <v>84375000</v>
+        <v>83625000</v>
       </c>
       <c r="W13" s="8" t="n">
         <f aca="false">T13</f>
-        <v>74375000</v>
+        <v>73625000</v>
       </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
@@ -1510,19 +1499,19 @@
       <c r="S14" s="8"/>
       <c r="T14" s="5" t="n">
         <f aca="false">T13+250000</f>
-        <v>74625000</v>
+        <v>73875000</v>
       </c>
       <c r="U14" s="6" t="n">
         <f aca="false">U13+250000</f>
-        <v>84625000</v>
+        <v>83875000</v>
       </c>
       <c r="V14" s="7" t="n">
         <f aca="false">U14</f>
-        <v>84625000</v>
+        <v>83875000</v>
       </c>
       <c r="W14" s="8" t="n">
         <f aca="false">T14</f>
-        <v>74625000</v>
+        <v>73875000</v>
       </c>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
@@ -1586,19 +1575,19 @@
       <c r="S15" s="8"/>
       <c r="T15" s="5" t="n">
         <f aca="false">T14+250000</f>
-        <v>74875000</v>
+        <v>74125000</v>
       </c>
       <c r="U15" s="6" t="n">
         <f aca="false">U14+250000</f>
-        <v>84875000</v>
+        <v>84125000</v>
       </c>
       <c r="V15" s="7" t="n">
         <f aca="false">U15</f>
-        <v>84875000</v>
+        <v>84125000</v>
       </c>
       <c r="W15" s="8" t="n">
         <f aca="false">T15</f>
-        <v>74875000</v>
+        <v>74125000</v>
       </c>
       <c r="X15" s="5"/>
       <c r="Y15" s="6"/>
@@ -1662,19 +1651,19 @@
       <c r="S16" s="8"/>
       <c r="T16" s="5" t="n">
         <f aca="false">T15+250000</f>
-        <v>75125000</v>
+        <v>74375000</v>
       </c>
       <c r="U16" s="6" t="n">
         <f aca="false">U15+250000</f>
-        <v>85125000</v>
+        <v>84375000</v>
       </c>
       <c r="V16" s="7" t="n">
         <f aca="false">U16</f>
-        <v>85125000</v>
+        <v>84375000</v>
       </c>
       <c r="W16" s="8" t="n">
         <f aca="false">T16</f>
-        <v>75125000</v>
+        <v>74375000</v>
       </c>
       <c r="X16" s="5"/>
       <c r="Y16" s="6"/>
@@ -1738,19 +1727,19 @@
       <c r="S17" s="8"/>
       <c r="T17" s="5" t="n">
         <f aca="false">T16+250000</f>
-        <v>75375000</v>
+        <v>74625000</v>
       </c>
       <c r="U17" s="6" t="n">
         <f aca="false">U16+250000</f>
-        <v>85375000</v>
+        <v>84625000</v>
       </c>
       <c r="V17" s="7" t="n">
         <f aca="false">U17</f>
-        <v>85375000</v>
+        <v>84625000</v>
       </c>
       <c r="W17" s="8" t="n">
         <f aca="false">T17</f>
-        <v>75375000</v>
+        <v>74625000</v>
       </c>
       <c r="X17" s="5"/>
       <c r="Y17" s="6"/>
@@ -1814,19 +1803,19 @@
       <c r="S18" s="8"/>
       <c r="T18" s="5" t="n">
         <f aca="false">T17+250000</f>
-        <v>75625000</v>
+        <v>74875000</v>
       </c>
       <c r="U18" s="6" t="n">
         <f aca="false">U17+250000</f>
-        <v>85625000</v>
+        <v>84875000</v>
       </c>
       <c r="V18" s="7" t="n">
         <f aca="false">U18</f>
-        <v>85625000</v>
+        <v>84875000</v>
       </c>
       <c r="W18" s="8" t="n">
         <f aca="false">T18</f>
-        <v>75625000</v>
+        <v>74875000</v>
       </c>
       <c r="X18" s="5"/>
       <c r="Y18" s="6"/>
@@ -1890,19 +1879,19 @@
       <c r="S19" s="8"/>
       <c r="T19" s="5" t="n">
         <f aca="false">T18+250000</f>
-        <v>75875000</v>
+        <v>75125000</v>
       </c>
       <c r="U19" s="6" t="n">
         <f aca="false">U18+250000</f>
-        <v>85875000</v>
+        <v>85125000</v>
       </c>
       <c r="V19" s="7" t="n">
         <f aca="false">U19</f>
-        <v>85875000</v>
+        <v>85125000</v>
       </c>
       <c r="W19" s="8" t="n">
         <f aca="false">T19</f>
-        <v>75875000</v>
+        <v>75125000</v>
       </c>
       <c r="X19" s="5"/>
       <c r="Y19" s="6"/>
@@ -1966,19 +1955,19 @@
       <c r="S20" s="8"/>
       <c r="T20" s="5" t="n">
         <f aca="false">T19+250000</f>
-        <v>76125000</v>
+        <v>75375000</v>
       </c>
       <c r="U20" s="6" t="n">
         <f aca="false">U19+250000</f>
-        <v>86125000</v>
+        <v>85375000</v>
       </c>
       <c r="V20" s="7" t="n">
         <f aca="false">U20</f>
-        <v>86125000</v>
+        <v>85375000</v>
       </c>
       <c r="W20" s="8" t="n">
         <f aca="false">T20</f>
-        <v>76125000</v>
+        <v>75375000</v>
       </c>
       <c r="X20" s="5"/>
       <c r="Y20" s="6"/>
@@ -2042,19 +2031,19 @@
       <c r="S21" s="8"/>
       <c r="T21" s="5" t="n">
         <f aca="false">T20+250000</f>
-        <v>76375000</v>
+        <v>75625000</v>
       </c>
       <c r="U21" s="6" t="n">
         <f aca="false">U20+250000</f>
-        <v>86375000</v>
+        <v>85625000</v>
       </c>
       <c r="V21" s="7" t="n">
         <f aca="false">U21</f>
-        <v>86375000</v>
+        <v>85625000</v>
       </c>
       <c r="W21" s="8" t="n">
         <f aca="false">T21</f>
-        <v>76375000</v>
+        <v>75625000</v>
       </c>
       <c r="X21" s="5"/>
       <c r="Y21" s="6"/>
@@ -2116,22 +2105,10 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="7"/>
       <c r="S22" s="8"/>
-      <c r="T22" s="5" t="n">
-        <f aca="false">T21+250000</f>
-        <v>76625000</v>
-      </c>
-      <c r="U22" s="6" t="n">
-        <f aca="false">U21+250000</f>
-        <v>86625000</v>
-      </c>
-      <c r="V22" s="7" t="n">
-        <f aca="false">U22</f>
-        <v>86625000</v>
-      </c>
-      <c r="W22" s="8" t="n">
-        <f aca="false">T22</f>
-        <v>76625000</v>
-      </c>
+      <c r="T22" s="5"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="8"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="6"/>
       <c r="Z22" s="7"/>
@@ -2192,22 +2169,10 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="7"/>
       <c r="S23" s="8"/>
-      <c r="T23" s="5" t="n">
-        <f aca="false">T22+250000</f>
-        <v>76875000</v>
-      </c>
-      <c r="U23" s="6" t="n">
-        <f aca="false">U22+250000</f>
-        <v>86875000</v>
-      </c>
-      <c r="V23" s="7" t="n">
-        <f aca="false">U23</f>
-        <v>86875000</v>
-      </c>
-      <c r="W23" s="8" t="n">
-        <f aca="false">T23</f>
-        <v>76875000</v>
-      </c>
+      <c r="T23" s="5"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="8"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="6"/>
       <c r="Z23" s="7"/>
@@ -2268,22 +2233,10 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="7"/>
       <c r="S24" s="8"/>
-      <c r="T24" s="5" t="n">
-        <f aca="false">T23+250000</f>
-        <v>77125000</v>
-      </c>
-      <c r="U24" s="6" t="n">
-        <f aca="false">U23+250000</f>
-        <v>87125000</v>
-      </c>
-      <c r="V24" s="7" t="n">
-        <f aca="false">U24</f>
-        <v>87125000</v>
-      </c>
-      <c r="W24" s="8" t="n">
-        <f aca="false">T24</f>
-        <v>77125000</v>
-      </c>
+      <c r="T24" s="5"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="8"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="6"/>
       <c r="Z24" s="7"/>

</xml_diff>

<commit_message>
feature : update the data from Ceragon
</commit_message>
<xml_diff>
--- a/03-WTP-PoC/code/apps/spectrum/exl2cmd/NextFrequency.xlsx
+++ b/03-WTP-PoC/code/apps/spectrum/exl2cmd/NextFrequency.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="1" state="visible" r:id="rId2"/>
@@ -74,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -110,19 +110,6 @@
       <color rgb="FFA6A6A6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -278,8 +265,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -298,15 +289,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,14 +376,14 @@
   </sheetPr>
   <dimension ref="B2:AMJ65535"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V22" activeCellId="0" sqref="V22:W24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.61860465116279"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3720930232558"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.68312757201646"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.761316872428"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,18 +526,18 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="n">
-        <v>14732000</v>
+        <v>14768000</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>15047000</v>
+        <v>15083000</v>
       </c>
       <c r="D4" s="7" t="n">
         <f aca="false">C4</f>
-        <v>15047000</v>
+        <v>15083000</v>
       </c>
       <c r="E4" s="8" t="n">
         <f aca="false">B4</f>
-        <v>14732000</v>
+        <v>14768000</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>21988250</v>
@@ -574,7 +561,7 @@
         <f aca="false">J4+10000000</f>
         <v>81156250</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="11" t="n">
         <v>72125000</v>
       </c>
       <c r="M4" s="6" t="n">
@@ -588,17 +575,17 @@
         <f aca="false">L4</f>
         <v>72125000</v>
       </c>
-      <c r="P4" s="11" t="n">
+      <c r="P4" s="12" t="n">
         <v>5960025</v>
       </c>
-      <c r="Q4" s="12" t="n">
+      <c r="Q4" s="13" t="n">
         <v>6212065</v>
       </c>
-      <c r="R4" s="11" t="n">
+      <c r="R4" s="12" t="n">
         <f aca="false">Q4</f>
         <v>6212065</v>
       </c>
-      <c r="S4" s="12" t="n">
+      <c r="S4" s="13" t="n">
         <f aca="false">P4</f>
         <v>5960025</v>
       </c>
@@ -634,19 +621,19 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="n">
         <f aca="false">B4+1000</f>
-        <v>14733000</v>
+        <v>14769000</v>
       </c>
       <c r="C5" s="6" t="n">
         <f aca="false">C4+1000</f>
-        <v>15048000</v>
+        <v>15084000</v>
       </c>
       <c r="D5" s="7" t="n">
         <f aca="false">C5</f>
-        <v>15048000</v>
+        <v>15084000</v>
       </c>
       <c r="E5" s="8" t="n">
         <f aca="false">B5</f>
-        <v>14733000</v>
+        <v>14769000</v>
       </c>
       <c r="F5" s="5" t="n">
         <f aca="false">F4+250000</f>
@@ -688,18 +675,18 @@
         <f aca="false">L5</f>
         <v>72375000</v>
       </c>
-      <c r="P5" s="13" t="n">
+      <c r="P5" s="14" t="n">
         <f aca="false">P4+250000</f>
         <v>6210025</v>
       </c>
-      <c r="Q5" s="14" t="n">
+      <c r="Q5" s="15" t="n">
         <v>6271365</v>
       </c>
-      <c r="R5" s="13" t="n">
+      <c r="R5" s="14" t="n">
         <f aca="false">Q5</f>
         <v>6271365</v>
       </c>
-      <c r="S5" s="14" t="n">
+      <c r="S5" s="15" t="n">
         <f aca="false">P5</f>
         <v>6210025</v>
       </c>
@@ -739,19 +726,19 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="n">
         <f aca="false">B5+1000</f>
-        <v>14734000</v>
+        <v>14770000</v>
       </c>
       <c r="C6" s="6" t="n">
         <f aca="false">C5+1000</f>
-        <v>15049000</v>
+        <v>15085000</v>
       </c>
       <c r="D6" s="7" t="n">
         <f aca="false">C6</f>
-        <v>15049000</v>
+        <v>15085000</v>
       </c>
       <c r="E6" s="8" t="n">
         <f aca="false">B6</f>
-        <v>14734000</v>
+        <v>14770000</v>
       </c>
       <c r="F6" s="5" t="n">
         <f aca="false">F5+250000</f>
@@ -793,17 +780,17 @@
         <f aca="false">L6</f>
         <v>72625000</v>
       </c>
-      <c r="P6" s="13" t="n">
+      <c r="P6" s="14" t="n">
         <v>6078625</v>
       </c>
-      <c r="Q6" s="14" t="n">
+      <c r="Q6" s="15" t="n">
         <v>6330665</v>
       </c>
-      <c r="R6" s="13" t="n">
+      <c r="R6" s="14" t="n">
         <f aca="false">Q6</f>
         <v>6330665</v>
       </c>
-      <c r="S6" s="14" t="n">
+      <c r="S6" s="15" t="n">
         <f aca="false">P6</f>
         <v>6078625</v>
       </c>
@@ -843,19 +830,19 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="n">
         <f aca="false">B6+1000</f>
-        <v>14735000</v>
+        <v>14771000</v>
       </c>
       <c r="C7" s="6" t="n">
         <f aca="false">C6+1000</f>
-        <v>15050000</v>
+        <v>15086000</v>
       </c>
       <c r="D7" s="7" t="n">
         <f aca="false">C7</f>
-        <v>15050000</v>
+        <v>15086000</v>
       </c>
       <c r="E7" s="8" t="n">
         <f aca="false">B7</f>
-        <v>14735000</v>
+        <v>14771000</v>
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">F6+250000</f>
@@ -881,7 +868,7 @@
         <f aca="false">J7+10000000</f>
         <v>81250000</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="16"/>
       <c r="N7" s="7" t="n">
         <f aca="false">M7</f>
@@ -891,17 +878,17 @@
         <f aca="false">L7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="13" t="n">
+      <c r="P7" s="14" t="n">
         <v>6137925</v>
       </c>
-      <c r="Q7" s="14" t="n">
+      <c r="Q7" s="15" t="n">
         <v>6389965</v>
       </c>
-      <c r="R7" s="13" t="n">
+      <c r="R7" s="14" t="n">
         <f aca="false">Q7</f>
         <v>6389965</v>
       </c>
-      <c r="S7" s="14" t="n">
+      <c r="S7" s="15" t="n">
         <f aca="false">P7</f>
         <v>6137925</v>
       </c>
@@ -941,19 +928,19 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="n">
         <f aca="false">B7+1000</f>
-        <v>14736000</v>
+        <v>14772000</v>
       </c>
       <c r="C8" s="6" t="n">
         <f aca="false">C7+1000</f>
-        <v>15051000</v>
+        <v>15087000</v>
       </c>
       <c r="D8" s="7" t="n">
         <f aca="false">C8</f>
-        <v>15051000</v>
+        <v>15087000</v>
       </c>
       <c r="E8" s="8" t="n">
         <f aca="false">B8</f>
-        <v>14736000</v>
+        <v>14772000</v>
       </c>
       <c r="F8" s="5" t="n">
         <f aca="false">F7+250000</f>
@@ -979,7 +966,7 @@
         <f aca="false">J8+10000000</f>
         <v>81281250</v>
       </c>
-      <c r="L8" s="15"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="16"/>
       <c r="N8" s="7" t="n">
         <f aca="false">M8</f>
@@ -1029,19 +1016,19 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="n">
         <f aca="false">B8+1000</f>
-        <v>14737000</v>
+        <v>14773000</v>
       </c>
       <c r="C9" s="6" t="n">
         <f aca="false">C8+1000</f>
-        <v>15052000</v>
+        <v>15088000</v>
       </c>
       <c r="D9" s="7" t="n">
         <f aca="false">C9</f>
-        <v>15052000</v>
+        <v>15088000</v>
       </c>
       <c r="E9" s="8" t="n">
         <f aca="false">B9</f>
-        <v>14737000</v>
+        <v>14773000</v>
       </c>
       <c r="F9" s="5" t="n">
         <f aca="false">F8+250000</f>
@@ -1067,7 +1054,7 @@
         <f aca="false">J9+10000000</f>
         <v>81312500</v>
       </c>
-      <c r="L9" s="15"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="16"/>
       <c r="N9" s="7" t="n">
         <f aca="false">M9</f>
@@ -1117,19 +1104,19 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="n">
         <f aca="false">B9+1000</f>
-        <v>14738000</v>
+        <v>14774000</v>
       </c>
       <c r="C10" s="6" t="n">
         <f aca="false">C9+1000</f>
-        <v>15053000</v>
+        <v>15089000</v>
       </c>
       <c r="D10" s="7" t="n">
         <f aca="false">C10</f>
-        <v>15053000</v>
+        <v>15089000</v>
       </c>
       <c r="E10" s="8" t="n">
         <f aca="false">B10</f>
-        <v>14738000</v>
+        <v>14774000</v>
       </c>
       <c r="F10" s="5" t="n">
         <f aca="false">F9+250000</f>
@@ -1155,7 +1142,7 @@
         <f aca="false">J10+10000000</f>
         <v>81343750</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="16"/>
       <c r="N10" s="7" t="n">
         <f aca="false">M10</f>
@@ -1205,19 +1192,19 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="n">
         <f aca="false">B10+1000</f>
-        <v>14739000</v>
+        <v>14775000</v>
       </c>
       <c r="C11" s="6" t="n">
         <f aca="false">C10+1000</f>
-        <v>15054000</v>
+        <v>15090000</v>
       </c>
       <c r="D11" s="7" t="n">
         <f aca="false">C11</f>
-        <v>15054000</v>
+        <v>15090000</v>
       </c>
       <c r="E11" s="8" t="n">
         <f aca="false">B11</f>
-        <v>14739000</v>
+        <v>14775000</v>
       </c>
       <c r="F11" s="5" t="n">
         <f aca="false">F10+250000</f>
@@ -1243,7 +1230,7 @@
         <f aca="false">J11+10000000</f>
         <v>81375000</v>
       </c>
-      <c r="L11" s="15"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="16"/>
       <c r="N11" s="7" t="n">
         <f aca="false">M11</f>
@@ -1293,19 +1280,19 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="n">
         <f aca="false">B11+1000</f>
-        <v>14740000</v>
+        <v>14776000</v>
       </c>
       <c r="C12" s="6" t="n">
         <f aca="false">C11+1000</f>
-        <v>15055000</v>
+        <v>15091000</v>
       </c>
       <c r="D12" s="7" t="n">
         <f aca="false">C12</f>
-        <v>15055000</v>
+        <v>15091000</v>
       </c>
       <c r="E12" s="8" t="n">
         <f aca="false">B12</f>
-        <v>14740000</v>
+        <v>14776000</v>
       </c>
       <c r="F12" s="5" t="n">
         <f aca="false">F11+250000</f>
@@ -1331,7 +1318,7 @@
         <f aca="false">J12+10000000</f>
         <v>81406250</v>
       </c>
-      <c r="L12" s="15"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="16"/>
       <c r="N12" s="7" t="n">
         <f aca="false">M12</f>
@@ -1369,19 +1356,19 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="n">
         <f aca="false">B12+1000</f>
-        <v>14741000</v>
+        <v>14777000</v>
       </c>
       <c r="C13" s="6" t="n">
         <f aca="false">C12+1000</f>
-        <v>15056000</v>
+        <v>15092000</v>
       </c>
       <c r="D13" s="7" t="n">
         <f aca="false">C13</f>
-        <v>15056000</v>
+        <v>15092000</v>
       </c>
       <c r="E13" s="8" t="n">
         <f aca="false">B13</f>
-        <v>14741000</v>
+        <v>14777000</v>
       </c>
       <c r="F13" s="5" t="n">
         <f aca="false">F12+250000</f>
@@ -1407,7 +1394,7 @@
         <f aca="false">J13+10000000</f>
         <v>81437500</v>
       </c>
-      <c r="L13" s="15"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="16"/>
       <c r="N13" s="7" t="n">
         <f aca="false">M13</f>
@@ -1445,19 +1432,19 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="n">
         <f aca="false">B13+1000</f>
-        <v>14742000</v>
+        <v>14778000</v>
       </c>
       <c r="C14" s="6" t="n">
         <f aca="false">C13+1000</f>
-        <v>15057000</v>
+        <v>15093000</v>
       </c>
       <c r="D14" s="7" t="n">
         <f aca="false">C14</f>
-        <v>15057000</v>
+        <v>15093000</v>
       </c>
       <c r="E14" s="8" t="n">
         <f aca="false">B14</f>
-        <v>14742000</v>
+        <v>14778000</v>
       </c>
       <c r="F14" s="5" t="n">
         <f aca="false">F13+250000</f>
@@ -1483,7 +1470,7 @@
         <f aca="false">J14+10000000</f>
         <v>81468750</v>
       </c>
-      <c r="L14" s="15"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="16"/>
       <c r="N14" s="7" t="n">
         <f aca="false">M14</f>
@@ -1521,19 +1508,19 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="n">
         <f aca="false">B14+1000</f>
-        <v>14743000</v>
+        <v>14779000</v>
       </c>
       <c r="C15" s="6" t="n">
         <f aca="false">C14+1000</f>
-        <v>15058000</v>
+        <v>15094000</v>
       </c>
       <c r="D15" s="7" t="n">
         <f aca="false">C15</f>
-        <v>15058000</v>
+        <v>15094000</v>
       </c>
       <c r="E15" s="8" t="n">
         <f aca="false">B15</f>
-        <v>14743000</v>
+        <v>14779000</v>
       </c>
       <c r="F15" s="5" t="n">
         <f aca="false">F14+250000</f>
@@ -1559,7 +1546,7 @@
         <f aca="false">J15+10000000</f>
         <v>81500000</v>
       </c>
-      <c r="L15" s="15"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="16"/>
       <c r="N15" s="7" t="n">
         <f aca="false">M15</f>
@@ -1597,19 +1584,19 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="n">
         <f aca="false">B15+1000</f>
-        <v>14744000</v>
+        <v>14780000</v>
       </c>
       <c r="C16" s="6" t="n">
         <f aca="false">C15+1000</f>
-        <v>15059000</v>
+        <v>15095000</v>
       </c>
       <c r="D16" s="7" t="n">
         <f aca="false">C16</f>
-        <v>15059000</v>
+        <v>15095000</v>
       </c>
       <c r="E16" s="8" t="n">
         <f aca="false">B16</f>
-        <v>14744000</v>
+        <v>14780000</v>
       </c>
       <c r="F16" s="5" t="n">
         <f aca="false">F15+250000</f>
@@ -1635,7 +1622,7 @@
         <f aca="false">J16+10000000</f>
         <v>81531250</v>
       </c>
-      <c r="L16" s="15"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="16"/>
       <c r="N16" s="7" t="n">
         <f aca="false">M16</f>
@@ -1673,19 +1660,19 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="n">
         <f aca="false">B16+1000</f>
-        <v>14745000</v>
+        <v>14781000</v>
       </c>
       <c r="C17" s="6" t="n">
         <f aca="false">C16+1000</f>
-        <v>15060000</v>
+        <v>15096000</v>
       </c>
       <c r="D17" s="7" t="n">
         <f aca="false">C17</f>
-        <v>15060000</v>
+        <v>15096000</v>
       </c>
       <c r="E17" s="8" t="n">
         <f aca="false">B17</f>
-        <v>14745000</v>
+        <v>14781000</v>
       </c>
       <c r="F17" s="5" t="n">
         <f aca="false">F16+250000</f>
@@ -1711,7 +1698,7 @@
         <f aca="false">J17+10000000</f>
         <v>81562500</v>
       </c>
-      <c r="L17" s="15"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="16"/>
       <c r="N17" s="7" t="n">
         <f aca="false">M17</f>
@@ -1749,19 +1736,19 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5" t="n">
         <f aca="false">B17+1000</f>
-        <v>14746000</v>
+        <v>14782000</v>
       </c>
       <c r="C18" s="6" t="n">
         <f aca="false">C17+1000</f>
-        <v>15061000</v>
+        <v>15097000</v>
       </c>
       <c r="D18" s="7" t="n">
         <f aca="false">C18</f>
-        <v>15061000</v>
+        <v>15097000</v>
       </c>
       <c r="E18" s="8" t="n">
         <f aca="false">B18</f>
-        <v>14746000</v>
+        <v>14782000</v>
       </c>
       <c r="F18" s="5" t="n">
         <f aca="false">F17+250000</f>
@@ -1787,7 +1774,7 @@
         <f aca="false">J18+10000000</f>
         <v>81593750</v>
       </c>
-      <c r="L18" s="15"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="16"/>
       <c r="N18" s="7" t="n">
         <f aca="false">M18</f>
@@ -1825,19 +1812,19 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5" t="n">
         <f aca="false">B18+1000</f>
-        <v>14747000</v>
+        <v>14783000</v>
       </c>
       <c r="C19" s="6" t="n">
         <f aca="false">C18+1000</f>
-        <v>15062000</v>
+        <v>15098000</v>
       </c>
       <c r="D19" s="7" t="n">
         <f aca="false">C19</f>
-        <v>15062000</v>
+        <v>15098000</v>
       </c>
       <c r="E19" s="8" t="n">
         <f aca="false">B19</f>
-        <v>14747000</v>
+        <v>14783000</v>
       </c>
       <c r="F19" s="5" t="n">
         <f aca="false">F18+250000</f>
@@ -1863,7 +1850,7 @@
         <f aca="false">J19+10000000</f>
         <v>81625000</v>
       </c>
-      <c r="L19" s="15"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="16"/>
       <c r="N19" s="7" t="n">
         <f aca="false">M19</f>
@@ -1901,19 +1888,19 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="n">
         <f aca="false">B19+1000</f>
-        <v>14748000</v>
+        <v>14784000</v>
       </c>
       <c r="C20" s="6" t="n">
         <f aca="false">C19+1000</f>
-        <v>15063000</v>
+        <v>15099000</v>
       </c>
       <c r="D20" s="7" t="n">
         <f aca="false">C20</f>
-        <v>15063000</v>
+        <v>15099000</v>
       </c>
       <c r="E20" s="8" t="n">
         <f aca="false">B20</f>
-        <v>14748000</v>
+        <v>14784000</v>
       </c>
       <c r="F20" s="5" t="n">
         <f aca="false">F19+250000</f>
@@ -1939,7 +1926,7 @@
         <f aca="false">J20+10000000</f>
         <v>81656250</v>
       </c>
-      <c r="L20" s="15"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="16"/>
       <c r="N20" s="7" t="n">
         <f aca="false">M20</f>
@@ -1977,19 +1964,19 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="n">
         <f aca="false">B20+1000</f>
-        <v>14749000</v>
+        <v>14785000</v>
       </c>
       <c r="C21" s="6" t="n">
         <f aca="false">C20+1000</f>
-        <v>15064000</v>
+        <v>15100000</v>
       </c>
       <c r="D21" s="7" t="n">
         <f aca="false">C21</f>
-        <v>15064000</v>
+        <v>15100000</v>
       </c>
       <c r="E21" s="8" t="n">
         <f aca="false">B21</f>
-        <v>14749000</v>
+        <v>14785000</v>
       </c>
       <c r="F21" s="5" t="n">
         <f aca="false">F20+250000</f>
@@ -2015,7 +2002,7 @@
         <f aca="false">J21+10000000</f>
         <v>81687500</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="16"/>
       <c r="N21" s="7" t="n">
         <f aca="false">M21</f>
@@ -2053,19 +2040,19 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="n">
         <f aca="false">B21+1000</f>
-        <v>14750000</v>
+        <v>14786000</v>
       </c>
       <c r="C22" s="6" t="n">
         <f aca="false">C21+1000</f>
-        <v>15065000</v>
+        <v>15101000</v>
       </c>
       <c r="D22" s="7" t="n">
         <f aca="false">C22</f>
-        <v>15065000</v>
+        <v>15101000</v>
       </c>
       <c r="E22" s="8" t="n">
         <f aca="false">B22</f>
-        <v>14750000</v>
+        <v>14786000</v>
       </c>
       <c r="F22" s="5" t="n">
         <f aca="false">F21+250000</f>
@@ -2091,7 +2078,7 @@
         <f aca="false">J22+10000000</f>
         <v>81718750</v>
       </c>
-      <c r="L22" s="15"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="16"/>
       <c r="N22" s="7" t="n">
         <f aca="false">M22</f>
@@ -2117,19 +2104,19 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="n">
         <f aca="false">B22+1000</f>
-        <v>14751000</v>
+        <v>14787000</v>
       </c>
       <c r="C23" s="6" t="n">
         <f aca="false">C22+1000</f>
-        <v>15066000</v>
+        <v>15102000</v>
       </c>
       <c r="D23" s="7" t="n">
         <f aca="false">C23</f>
-        <v>15066000</v>
+        <v>15102000</v>
       </c>
       <c r="E23" s="8" t="n">
         <f aca="false">B23</f>
-        <v>14751000</v>
+        <v>14787000</v>
       </c>
       <c r="F23" s="5" t="n">
         <f aca="false">F22+250000</f>
@@ -2155,7 +2142,7 @@
         <f aca="false">J23+10000000</f>
         <v>81750000</v>
       </c>
-      <c r="L23" s="15"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="16"/>
       <c r="N23" s="7" t="n">
         <f aca="false">M23</f>
@@ -2181,19 +2168,19 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="n">
         <f aca="false">B23+1000</f>
-        <v>14752000</v>
+        <v>14788000</v>
       </c>
       <c r="C24" s="6" t="n">
         <f aca="false">C23+1000</f>
-        <v>15067000</v>
+        <v>15103000</v>
       </c>
       <c r="D24" s="7" t="n">
         <f aca="false">C24</f>
-        <v>15067000</v>
+        <v>15103000</v>
       </c>
       <c r="E24" s="8" t="n">
         <f aca="false">B24</f>
-        <v>14752000</v>
+        <v>14788000</v>
       </c>
       <c r="F24" s="5" t="n">
         <f aca="false">F23+250000</f>
@@ -2219,7 +2206,7 @@
         <f aca="false">J24+10000000</f>
         <v>82000000</v>
       </c>
-      <c r="L24" s="15"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="16"/>
       <c r="N24" s="7" t="n">
         <f aca="false">M24</f>
@@ -2281,7 +2268,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>